<commit_message>
add optin to upload file from manager
</commit_message>
<xml_diff>
--- a/assets/‏‏29.3.24.xlsx
+++ b/assets/‏‏29.3.24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\Siduration\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9A56EF-DB24-4F45-A7FB-0B84AEEE66E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DBCDE7-0D1C-471C-8740-4AFDBFFAA311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31650" yWindow="2850" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3330" yWindow="3495" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>FirstName</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>AmountInvited</t>
+  </si>
+  <si>
+    <t>DoSendMessage</t>
   </si>
 </sst>
 </file>
@@ -694,7 +697,7 @@
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -704,9 +707,9 @@
     <col min="3" max="3" width="12.625" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.75" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" customWidth="1"/>
+    <col min="8" max="8" width="17.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
@@ -731,7 +734,9 @@
       <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="23"/>
+      <c r="H1" s="23" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">

</xml_diff>